<commit_message>
Exclude internal from formatted
</commit_message>
<xml_diff>
--- a/output/Kenya_formatted.xlsx
+++ b/output/Kenya_formatted.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="234">
   <si>
     <t xml:space="preserve">Country Code</t>
   </si>
@@ -624,9 +624,6 @@
   </si>
   <si>
     <t xml:space="preserve">Adm support  (USAID/OFDA)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Support to: (i) treatment of Moderate Acute Malnutrition (MAM) among children 6-59 months, and pregnant and lactating women; and (ii) prevention of deterioration in the nutrition status of children 6-59 months.</t>
   </si>
   <si>
     <t xml:space="preserve">Support to drought affected population to decrease food insecurity and malnutrition</t>
@@ -12176,29 +12173,33 @@
         <v>41</v>
       </c>
       <c r="E108" t="s">
-        <v>121</v>
+        <v>66</v>
       </c>
       <c r="F108"/>
       <c r="G108" s="1" t="n">
-        <v>43026</v>
+        <v>43027</v>
       </c>
       <c r="H108" s="1" t="n">
-        <v>43089</v>
+        <v>43160</v>
       </c>
       <c r="I108" t="s">
-        <v>168</v>
+        <v>204</v>
       </c>
       <c r="J108" t="s">
         <v>44</v>
       </c>
-      <c r="K108"/>
-      <c r="L108"/>
+      <c r="K108" t="n">
+        <v>2</v>
+      </c>
+      <c r="L108" t="n">
+        <v>8.131</v>
+      </c>
       <c r="M108" t="n">
-        <v>49.301049</v>
+        <v>0.245972</v>
       </c>
       <c r="N108"/>
       <c r="O108" t="n">
-        <v>49.301049</v>
+        <v>0.245972</v>
       </c>
       <c r="P108" t="n">
         <v>1</v>
@@ -12231,7 +12232,7 @@
         <v>0</v>
       </c>
       <c r="Z108" t="n">
-        <v>49.301049</v>
+        <v>0.245972</v>
       </c>
       <c r="AA108" t="n">
         <v>0</v>
@@ -12252,7 +12253,7 @@
         <v>0</v>
       </c>
       <c r="AG108" t="n">
-        <v>49.301049</v>
+        <v>0.245972</v>
       </c>
       <c r="AH108"/>
       <c r="AI108"/>
@@ -12261,7 +12262,7 @@
         <v>0</v>
       </c>
       <c r="AL108" t="n">
-        <v>165051</v>
+        <v>171123</v>
       </c>
     </row>
     <row r="109">
@@ -12278,29 +12279,33 @@
         <v>41</v>
       </c>
       <c r="E109" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="F109"/>
       <c r="G109" s="1" t="n">
-        <v>43026</v>
+        <v>43035</v>
       </c>
       <c r="H109" s="1" t="n">
         <v>43089</v>
       </c>
       <c r="I109" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="J109" t="s">
-        <v>44</v>
-      </c>
-      <c r="K109"/>
-      <c r="L109"/>
+        <v>206</v>
+      </c>
+      <c r="K109" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="L109" t="n">
+        <v>0.848</v>
+      </c>
       <c r="M109" t="n">
-        <v>22.387468</v>
+        <v>4.127358</v>
       </c>
       <c r="N109"/>
       <c r="O109" t="n">
-        <v>22.387468</v>
+        <v>4.127358</v>
       </c>
       <c r="P109" t="n">
         <v>1</v>
@@ -12333,7 +12338,7 @@
         <v>0</v>
       </c>
       <c r="Z109" t="n">
-        <v>22.387468</v>
+        <v>4.127358</v>
       </c>
       <c r="AA109" t="n">
         <v>0</v>
@@ -12354,7 +12359,7 @@
         <v>0</v>
       </c>
       <c r="AG109" t="n">
-        <v>22.387468</v>
+        <v>4.127358</v>
       </c>
       <c r="AH109"/>
       <c r="AI109"/>
@@ -12363,7 +12368,7 @@
         <v>0</v>
       </c>
       <c r="AL109" t="n">
-        <v>165052</v>
+        <v>165523</v>
       </c>
     </row>
     <row r="110">
@@ -12380,33 +12385,29 @@
         <v>41</v>
       </c>
       <c r="E110" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="F110"/>
       <c r="G110" s="1" t="n">
-        <v>43027</v>
+        <v>43048</v>
       </c>
       <c r="H110" s="1" t="n">
-        <v>43160</v>
+        <v>43089</v>
       </c>
       <c r="I110" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="J110" t="s">
-        <v>44</v>
-      </c>
-      <c r="K110" t="n">
-        <v>2</v>
-      </c>
-      <c r="L110" t="n">
-        <v>8.131</v>
-      </c>
+        <v>207</v>
+      </c>
+      <c r="K110"/>
+      <c r="L110"/>
       <c r="M110" t="n">
-        <v>0.245972</v>
+        <v>5.666384</v>
       </c>
       <c r="N110"/>
       <c r="O110" t="n">
-        <v>0.245972</v>
+        <v>5.666384</v>
       </c>
       <c r="P110" t="n">
         <v>1</v>
@@ -12439,10 +12440,10 @@
         <v>0</v>
       </c>
       <c r="Z110" t="n">
-        <v>0.245972</v>
+        <v>0</v>
       </c>
       <c r="AA110" t="n">
-        <v>0</v>
+        <v>5.666384</v>
       </c>
       <c r="AB110" t="n">
         <v>0</v>
@@ -12460,7 +12461,7 @@
         <v>0</v>
       </c>
       <c r="AG110" t="n">
-        <v>0.245972</v>
+        <v>5.666384</v>
       </c>
       <c r="AH110"/>
       <c r="AI110"/>
@@ -12469,7 +12470,7 @@
         <v>0</v>
       </c>
       <c r="AL110" t="n">
-        <v>171123</v>
+        <v>168260</v>
       </c>
     </row>
     <row r="111">
@@ -12486,33 +12487,29 @@
         <v>41</v>
       </c>
       <c r="E111" t="s">
-        <v>136</v>
+        <v>49</v>
       </c>
       <c r="F111"/>
       <c r="G111" s="1" t="n">
-        <v>43035</v>
+        <v>43048</v>
       </c>
       <c r="H111" s="1" t="n">
         <v>43089</v>
       </c>
       <c r="I111" t="s">
-        <v>206</v>
+        <v>168</v>
       </c>
       <c r="J111" t="s">
-        <v>207</v>
-      </c>
-      <c r="K111" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="L111" t="n">
-        <v>0.848</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="K111"/>
+      <c r="L111"/>
       <c r="M111" t="n">
-        <v>4.127358</v>
+        <v>7.494975</v>
       </c>
       <c r="N111"/>
       <c r="O111" t="n">
-        <v>4.127358</v>
+        <v>7.494975</v>
       </c>
       <c r="P111" t="n">
         <v>1</v>
@@ -12545,10 +12542,10 @@
         <v>0</v>
       </c>
       <c r="Z111" t="n">
-        <v>4.127358</v>
+        <v>0</v>
       </c>
       <c r="AA111" t="n">
-        <v>0</v>
+        <v>7.494975</v>
       </c>
       <c r="AB111" t="n">
         <v>0</v>
@@ -12566,7 +12563,7 @@
         <v>0</v>
       </c>
       <c r="AG111" t="n">
-        <v>4.127358</v>
+        <v>7.494975</v>
       </c>
       <c r="AH111"/>
       <c r="AI111"/>
@@ -12575,7 +12572,7 @@
         <v>0</v>
       </c>
       <c r="AL111" t="n">
-        <v>165523</v>
+        <v>168261</v>
       </c>
     </row>
     <row r="112">
@@ -12592,29 +12589,33 @@
         <v>41</v>
       </c>
       <c r="E112" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="F112"/>
       <c r="G112" s="1" t="n">
-        <v>43048</v>
+        <v>43058</v>
       </c>
       <c r="H112" s="1" t="n">
-        <v>43089</v>
+        <v>43088</v>
       </c>
       <c r="I112" t="s">
-        <v>168</v>
+        <v>209</v>
       </c>
       <c r="J112" t="s">
-        <v>208</v>
-      </c>
-      <c r="K112"/>
-      <c r="L112"/>
+        <v>44</v>
+      </c>
+      <c r="K112" t="n">
+        <v>2</v>
+      </c>
+      <c r="L112" t="n">
+        <v>8.36</v>
+      </c>
       <c r="M112" t="n">
-        <v>5.666384</v>
+        <v>0.239234</v>
       </c>
       <c r="N112"/>
       <c r="O112" t="n">
-        <v>5.666384</v>
+        <v>0.239234</v>
       </c>
       <c r="P112" t="n">
         <v>1</v>
@@ -12650,7 +12651,7 @@
         <v>0</v>
       </c>
       <c r="AA112" t="n">
-        <v>5.666384</v>
+        <v>0.239234</v>
       </c>
       <c r="AB112" t="n">
         <v>0</v>
@@ -12668,7 +12669,7 @@
         <v>0</v>
       </c>
       <c r="AG112" t="n">
-        <v>5.666384</v>
+        <v>0.239234</v>
       </c>
       <c r="AH112"/>
       <c r="AI112"/>
@@ -12677,7 +12678,7 @@
         <v>0</v>
       </c>
       <c r="AL112" t="n">
-        <v>168260</v>
+        <v>168142</v>
       </c>
     </row>
     <row r="113">
@@ -12698,25 +12699,25 @@
       </c>
       <c r="F113"/>
       <c r="G113" s="1" t="n">
-        <v>43048</v>
+        <v>43061</v>
       </c>
       <c r="H113" s="1" t="n">
-        <v>43089</v>
+        <v>43286</v>
       </c>
       <c r="I113" t="s">
-        <v>168</v>
+        <v>210</v>
       </c>
       <c r="J113" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="K113"/>
       <c r="L113"/>
       <c r="M113" t="n">
-        <v>7.494975</v>
+        <v>5.988165</v>
       </c>
       <c r="N113"/>
       <c r="O113" t="n">
-        <v>7.494975</v>
+        <v>5.988165</v>
       </c>
       <c r="P113" t="n">
         <v>1</v>
@@ -12752,7 +12753,7 @@
         <v>0</v>
       </c>
       <c r="AA113" t="n">
-        <v>7.494975</v>
+        <v>5.988165</v>
       </c>
       <c r="AB113" t="n">
         <v>0</v>
@@ -12770,7 +12771,7 @@
         <v>0</v>
       </c>
       <c r="AG113" t="n">
-        <v>7.494975</v>
+        <v>5.988165</v>
       </c>
       <c r="AH113"/>
       <c r="AI113"/>
@@ -12779,7 +12780,7 @@
         <v>0</v>
       </c>
       <c r="AL113" t="n">
-        <v>168261</v>
+        <v>174568</v>
       </c>
     </row>
     <row r="114">
@@ -12796,33 +12797,29 @@
         <v>41</v>
       </c>
       <c r="E114" t="s">
-        <v>66</v>
+        <v>212</v>
       </c>
       <c r="F114"/>
       <c r="G114" s="1" t="n">
-        <v>43058</v>
+        <v>43062</v>
       </c>
       <c r="H114" s="1" t="n">
-        <v>43088</v>
+        <v>43133</v>
       </c>
       <c r="I114" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="J114" t="s">
-        <v>44</v>
-      </c>
-      <c r="K114" t="n">
-        <v>2</v>
-      </c>
-      <c r="L114" t="n">
-        <v>8.36</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="K114"/>
+      <c r="L114"/>
       <c r="M114" t="n">
-        <v>0.239234</v>
+        <v>0.058072</v>
       </c>
       <c r="N114"/>
       <c r="O114" t="n">
-        <v>0.239234</v>
+        <v>0.058072</v>
       </c>
       <c r="P114" t="n">
         <v>1</v>
@@ -12858,7 +12855,7 @@
         <v>0</v>
       </c>
       <c r="AA114" t="n">
-        <v>0.239234</v>
+        <v>0.058072</v>
       </c>
       <c r="AB114" t="n">
         <v>0</v>
@@ -12876,7 +12873,7 @@
         <v>0</v>
       </c>
       <c r="AG114" t="n">
-        <v>0.239234</v>
+        <v>0.058072</v>
       </c>
       <c r="AH114"/>
       <c r="AI114"/>
@@ -12885,7 +12882,7 @@
         <v>0</v>
       </c>
       <c r="AL114" t="n">
-        <v>168142</v>
+        <v>170171</v>
       </c>
     </row>
     <row r="115">
@@ -12902,29 +12899,29 @@
         <v>41</v>
       </c>
       <c r="E115" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="F115"/>
       <c r="G115" s="1" t="n">
-        <v>43061</v>
+        <v>43063</v>
       </c>
       <c r="H115" s="1" t="n">
-        <v>43286</v>
+        <v>43089</v>
       </c>
       <c r="I115" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="J115" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="K115"/>
       <c r="L115"/>
       <c r="M115" t="n">
-        <v>5.988165</v>
+        <v>13.192612</v>
       </c>
       <c r="N115"/>
       <c r="O115" t="n">
-        <v>5.988165</v>
+        <v>13.192612</v>
       </c>
       <c r="P115" t="n">
         <v>1</v>
@@ -12960,7 +12957,7 @@
         <v>0</v>
       </c>
       <c r="AA115" t="n">
-        <v>5.988165</v>
+        <v>13.192612</v>
       </c>
       <c r="AB115" t="n">
         <v>0</v>
@@ -12978,7 +12975,7 @@
         <v>0</v>
       </c>
       <c r="AG115" t="n">
-        <v>5.988165</v>
+        <v>13.192612</v>
       </c>
       <c r="AH115"/>
       <c r="AI115"/>
@@ -12987,7 +12984,7 @@
         <v>0</v>
       </c>
       <c r="AL115" t="n">
-        <v>174568</v>
+        <v>168257</v>
       </c>
     </row>
     <row r="116">
@@ -13004,29 +13001,29 @@
         <v>41</v>
       </c>
       <c r="E116" t="s">
-        <v>213</v>
+        <v>49</v>
       </c>
       <c r="F116"/>
       <c r="G116" s="1" t="n">
-        <v>43062</v>
+        <v>43069</v>
       </c>
       <c r="H116" s="1" t="n">
-        <v>43133</v>
+        <v>43286</v>
       </c>
       <c r="I116" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="J116" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K116"/>
       <c r="L116"/>
       <c r="M116" t="n">
-        <v>0.058072</v>
+        <v>27.988534</v>
       </c>
       <c r="N116"/>
       <c r="O116" t="n">
-        <v>0.058072</v>
+        <v>27.988534</v>
       </c>
       <c r="P116" t="n">
         <v>1</v>
@@ -13062,7 +13059,7 @@
         <v>0</v>
       </c>
       <c r="AA116" t="n">
-        <v>0.058072</v>
+        <v>27.988534</v>
       </c>
       <c r="AB116" t="n">
         <v>0</v>
@@ -13080,7 +13077,7 @@
         <v>0</v>
       </c>
       <c r="AG116" t="n">
-        <v>0.058072</v>
+        <v>27.988534</v>
       </c>
       <c r="AH116"/>
       <c r="AI116"/>
@@ -13089,7 +13086,7 @@
         <v>0</v>
       </c>
       <c r="AL116" t="n">
-        <v>170171</v>
+        <v>174569</v>
       </c>
     </row>
     <row r="117">
@@ -13106,29 +13103,33 @@
         <v>41</v>
       </c>
       <c r="E117" t="s">
-        <v>115</v>
+        <v>92</v>
       </c>
       <c r="F117"/>
       <c r="G117" s="1" t="n">
-        <v>43063</v>
+        <v>43147</v>
       </c>
       <c r="H117" s="1" t="n">
-        <v>43089</v>
+        <v>43650</v>
       </c>
       <c r="I117" t="s">
-        <v>168</v>
+        <v>217</v>
       </c>
       <c r="J117" t="s">
-        <v>216</v>
-      </c>
-      <c r="K117"/>
-      <c r="L117"/>
+        <v>218</v>
+      </c>
+      <c r="K117" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="L117" t="n">
+        <v>0.805</v>
+      </c>
       <c r="M117" t="n">
-        <v>13.192612</v>
+        <v>0.869565</v>
       </c>
       <c r="N117"/>
       <c r="O117" t="n">
-        <v>13.192612</v>
+        <v>0.869565</v>
       </c>
       <c r="P117" t="n">
         <v>1</v>
@@ -13164,10 +13165,10 @@
         <v>0</v>
       </c>
       <c r="AA117" t="n">
-        <v>13.192612</v>
+        <v>0</v>
       </c>
       <c r="AB117" t="n">
-        <v>0</v>
+        <v>0.869565</v>
       </c>
       <c r="AC117" t="n">
         <v>0</v>
@@ -13182,7 +13183,7 @@
         <v>0</v>
       </c>
       <c r="AG117" t="n">
-        <v>13.192612</v>
+        <v>0.869565</v>
       </c>
       <c r="AH117"/>
       <c r="AI117"/>
@@ -13191,7 +13192,7 @@
         <v>0</v>
       </c>
       <c r="AL117" t="n">
-        <v>168257</v>
+        <v>170854</v>
       </c>
     </row>
     <row r="118">
@@ -13208,29 +13209,33 @@
         <v>41</v>
       </c>
       <c r="E118" t="s">
-        <v>49</v>
+        <v>132</v>
       </c>
       <c r="F118"/>
       <c r="G118" s="1" t="n">
-        <v>43069</v>
+        <v>43150</v>
       </c>
       <c r="H118" s="1" t="n">
-        <v>43286</v>
+        <v>43151</v>
       </c>
       <c r="I118" t="s">
-        <v>211</v>
+        <v>219</v>
       </c>
       <c r="J118" t="s">
-        <v>217</v>
-      </c>
-      <c r="K118"/>
-      <c r="L118"/>
+        <v>220</v>
+      </c>
+      <c r="K118" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="L118" t="n">
+        <v>0.805</v>
+      </c>
       <c r="M118" t="n">
-        <v>27.988534</v>
+        <v>0.621118</v>
       </c>
       <c r="N118"/>
       <c r="O118" t="n">
-        <v>27.988534</v>
+        <v>0.621118</v>
       </c>
       <c r="P118" t="n">
         <v>1</v>
@@ -13266,10 +13271,10 @@
         <v>0</v>
       </c>
       <c r="AA118" t="n">
-        <v>27.988534</v>
+        <v>0</v>
       </c>
       <c r="AB118" t="n">
-        <v>0</v>
+        <v>0.621118</v>
       </c>
       <c r="AC118" t="n">
         <v>0</v>
@@ -13284,7 +13289,7 @@
         <v>0</v>
       </c>
       <c r="AG118" t="n">
-        <v>27.988534</v>
+        <v>0.621118</v>
       </c>
       <c r="AH118"/>
       <c r="AI118"/>
@@ -13293,7 +13298,7 @@
         <v>0</v>
       </c>
       <c r="AL118" t="n">
-        <v>174569</v>
+        <v>170825</v>
       </c>
     </row>
     <row r="119">
@@ -13310,33 +13315,33 @@
         <v>41</v>
       </c>
       <c r="E119" t="s">
-        <v>92</v>
+        <v>132</v>
       </c>
       <c r="F119"/>
       <c r="G119" s="1" t="n">
-        <v>43147</v>
+        <v>43153</v>
       </c>
       <c r="H119" s="1" t="n">
-        <v>43650</v>
+        <v>43154</v>
       </c>
       <c r="I119" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="J119" t="s">
-        <v>219</v>
+        <v>44</v>
       </c>
       <c r="K119" t="n">
-        <v>0.7</v>
+        <v>0.169</v>
       </c>
       <c r="L119" t="n">
         <v>0.805</v>
       </c>
       <c r="M119" t="n">
-        <v>0.869565</v>
+        <v>0.209938</v>
       </c>
       <c r="N119"/>
       <c r="O119" t="n">
-        <v>0.869565</v>
+        <v>0.209938</v>
       </c>
       <c r="P119" t="n">
         <v>1</v>
@@ -13375,7 +13380,7 @@
         <v>0</v>
       </c>
       <c r="AB119" t="n">
-        <v>0.869565</v>
+        <v>0.209938</v>
       </c>
       <c r="AC119" t="n">
         <v>0</v>
@@ -13390,7 +13395,7 @@
         <v>0</v>
       </c>
       <c r="AG119" t="n">
-        <v>0.869565</v>
+        <v>0.209938</v>
       </c>
       <c r="AH119"/>
       <c r="AI119"/>
@@ -13399,7 +13404,7 @@
         <v>0</v>
       </c>
       <c r="AL119" t="n">
-        <v>170854</v>
+        <v>170968</v>
       </c>
     </row>
     <row r="120">
@@ -13416,33 +13421,29 @@
         <v>41</v>
       </c>
       <c r="E120" t="s">
-        <v>132</v>
+        <v>49</v>
       </c>
       <c r="F120"/>
       <c r="G120" s="1" t="n">
-        <v>43150</v>
+        <v>43165</v>
       </c>
       <c r="H120" s="1" t="n">
-        <v>43151</v>
+        <v>43179</v>
       </c>
       <c r="I120" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="J120" t="s">
-        <v>221</v>
-      </c>
-      <c r="K120" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L120" t="n">
-        <v>0.805</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="K120"/>
+      <c r="L120"/>
       <c r="M120" t="n">
-        <v>0.621118</v>
+        <v>0.008037</v>
       </c>
       <c r="N120"/>
       <c r="O120" t="n">
-        <v>0.621118</v>
+        <v>0.008037</v>
       </c>
       <c r="P120" t="n">
         <v>1</v>
@@ -13481,10 +13482,10 @@
         <v>0</v>
       </c>
       <c r="AB120" t="n">
-        <v>0.621118</v>
+        <v>0</v>
       </c>
       <c r="AC120" t="n">
-        <v>0</v>
+        <v>0.008037</v>
       </c>
       <c r="AD120" t="n">
         <v>0</v>
@@ -13496,7 +13497,7 @@
         <v>0</v>
       </c>
       <c r="AG120" t="n">
-        <v>0.621118</v>
+        <v>0.008037</v>
       </c>
       <c r="AH120"/>
       <c r="AI120"/>
@@ -13505,7 +13506,7 @@
         <v>0</v>
       </c>
       <c r="AL120" t="n">
-        <v>170825</v>
+        <v>171709</v>
       </c>
     </row>
     <row r="121">
@@ -13522,33 +13523,33 @@
         <v>41</v>
       </c>
       <c r="E121" t="s">
-        <v>132</v>
+        <v>58</v>
       </c>
       <c r="F121"/>
       <c r="G121" s="1" t="n">
-        <v>43153</v>
+        <v>43168</v>
       </c>
       <c r="H121" s="1" t="n">
-        <v>43154</v>
+        <v>43237</v>
       </c>
       <c r="I121" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J121" t="s">
-        <v>44</v>
+        <v>224</v>
       </c>
       <c r="K121" t="n">
-        <v>0.169</v>
+        <v>1.25</v>
       </c>
       <c r="L121" t="n">
-        <v>0.805</v>
+        <v>6.071</v>
       </c>
       <c r="M121" t="n">
-        <v>0.209938</v>
+        <v>0.205897</v>
       </c>
       <c r="N121"/>
       <c r="O121" t="n">
-        <v>0.209938</v>
+        <v>0.205897</v>
       </c>
       <c r="P121" t="n">
         <v>1</v>
@@ -13587,10 +13588,10 @@
         <v>0</v>
       </c>
       <c r="AB121" t="n">
-        <v>0.209938</v>
+        <v>0</v>
       </c>
       <c r="AC121" t="n">
-        <v>0</v>
+        <v>0.205897</v>
       </c>
       <c r="AD121" t="n">
         <v>0</v>
@@ -13602,7 +13603,7 @@
         <v>0</v>
       </c>
       <c r="AG121" t="n">
-        <v>0.209938</v>
+        <v>0.205897</v>
       </c>
       <c r="AH121"/>
       <c r="AI121"/>
@@ -13611,7 +13612,7 @@
         <v>0</v>
       </c>
       <c r="AL121" t="n">
-        <v>170968</v>
+        <v>174617</v>
       </c>
     </row>
     <row r="122">
@@ -13628,29 +13629,33 @@
         <v>41</v>
       </c>
       <c r="E122" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="F122"/>
       <c r="G122" s="1" t="n">
-        <v>43165</v>
+        <v>43173</v>
       </c>
       <c r="H122" s="1" t="n">
-        <v>43179</v>
+        <v>43655</v>
       </c>
       <c r="I122" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="J122" t="s">
-        <v>44</v>
-      </c>
-      <c r="K122"/>
-      <c r="L122"/>
+        <v>226</v>
+      </c>
+      <c r="K122" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="L122" t="n">
+        <v>0.815</v>
+      </c>
       <c r="M122" t="n">
-        <v>0.008037</v>
+        <v>2.208589</v>
       </c>
       <c r="N122"/>
       <c r="O122" t="n">
-        <v>0.008037</v>
+        <v>2.208589</v>
       </c>
       <c r="P122" t="n">
         <v>1</v>
@@ -13692,7 +13697,7 @@
         <v>0</v>
       </c>
       <c r="AC122" t="n">
-        <v>0.008037</v>
+        <v>2.208589</v>
       </c>
       <c r="AD122" t="n">
         <v>0</v>
@@ -13704,7 +13709,7 @@
         <v>0</v>
       </c>
       <c r="AG122" t="n">
-        <v>0.008037</v>
+        <v>2.208589</v>
       </c>
       <c r="AH122"/>
       <c r="AI122"/>
@@ -13713,7 +13718,7 @@
         <v>0</v>
       </c>
       <c r="AL122" t="n">
-        <v>171709</v>
+        <v>171631</v>
       </c>
     </row>
     <row r="123">
@@ -13730,33 +13735,33 @@
         <v>41</v>
       </c>
       <c r="E123" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="F123"/>
       <c r="G123" s="1" t="n">
-        <v>43168</v>
+        <v>43173</v>
       </c>
       <c r="H123" s="1" t="n">
-        <v>43237</v>
+        <v>43703</v>
       </c>
       <c r="I123" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="J123" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="K123" t="n">
-        <v>1.25</v>
+        <v>0.667737</v>
       </c>
       <c r="L123" t="n">
-        <v>6.071</v>
+        <v>0.815</v>
       </c>
       <c r="M123" t="n">
-        <v>0.205897</v>
+        <v>0.819309</v>
       </c>
       <c r="N123"/>
       <c r="O123" t="n">
-        <v>0.205897</v>
+        <v>0.819309</v>
       </c>
       <c r="P123" t="n">
         <v>1</v>
@@ -13798,7 +13803,7 @@
         <v>0</v>
       </c>
       <c r="AC123" t="n">
-        <v>0.205897</v>
+        <v>0.819309</v>
       </c>
       <c r="AD123" t="n">
         <v>0</v>
@@ -13810,7 +13815,7 @@
         <v>0</v>
       </c>
       <c r="AG123" t="n">
-        <v>0.205897</v>
+        <v>0.819309</v>
       </c>
       <c r="AH123"/>
       <c r="AI123"/>
@@ -13819,7 +13824,7 @@
         <v>0</v>
       </c>
       <c r="AL123" t="n">
-        <v>174617</v>
+        <v>195291</v>
       </c>
     </row>
     <row r="124">
@@ -13836,33 +13841,33 @@
         <v>41</v>
       </c>
       <c r="E124" t="s">
-        <v>92</v>
+        <v>227</v>
       </c>
       <c r="F124"/>
       <c r="G124" s="1" t="n">
-        <v>43173</v>
+        <v>43251</v>
       </c>
       <c r="H124" s="1" t="n">
-        <v>43655</v>
+        <v>43263</v>
       </c>
       <c r="I124" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="J124" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="K124" t="n">
-        <v>1.8</v>
+        <v>0.2</v>
       </c>
       <c r="L124" t="n">
-        <v>0.815</v>
+        <v>0.99</v>
       </c>
       <c r="M124" t="n">
-        <v>2.208589</v>
+        <v>0.20202</v>
       </c>
       <c r="N124"/>
       <c r="O124" t="n">
-        <v>2.208589</v>
+        <v>0.20202</v>
       </c>
       <c r="P124" t="n">
         <v>1</v>
@@ -13904,10 +13909,10 @@
         <v>0</v>
       </c>
       <c r="AC124" t="n">
-        <v>2.208589</v>
+        <v>0</v>
       </c>
       <c r="AD124" t="n">
-        <v>0</v>
+        <v>0.20202</v>
       </c>
       <c r="AE124" t="n">
         <v>0</v>
@@ -13916,7 +13921,7 @@
         <v>0</v>
       </c>
       <c r="AG124" t="n">
-        <v>2.208589</v>
+        <v>0.20202</v>
       </c>
       <c r="AH124"/>
       <c r="AI124"/>
@@ -13925,7 +13930,7 @@
         <v>0</v>
       </c>
       <c r="AL124" t="n">
-        <v>171631</v>
+        <v>176336</v>
       </c>
     </row>
     <row r="125">
@@ -13942,33 +13947,29 @@
         <v>41</v>
       </c>
       <c r="E125" t="s">
-        <v>92</v>
+        <v>49</v>
       </c>
       <c r="F125"/>
       <c r="G125" s="1" t="n">
-        <v>43173</v>
+        <v>43259</v>
       </c>
       <c r="H125" s="1" t="n">
-        <v>43703</v>
+        <v>43332</v>
       </c>
       <c r="I125" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
       <c r="J125" t="s">
-        <v>227</v>
-      </c>
-      <c r="K125" t="n">
-        <v>0.667737</v>
-      </c>
-      <c r="L125" t="n">
-        <v>0.815</v>
-      </c>
+        <v>231</v>
+      </c>
+      <c r="K125"/>
+      <c r="L125"/>
       <c r="M125" t="n">
-        <v>0.819309</v>
+        <v>1.5</v>
       </c>
       <c r="N125"/>
       <c r="O125" t="n">
-        <v>0.819309</v>
+        <v>1.5</v>
       </c>
       <c r="P125" t="n">
         <v>1</v>
@@ -14010,19 +14011,19 @@
         <v>0</v>
       </c>
       <c r="AC125" t="n">
-        <v>0.819309</v>
+        <v>0</v>
       </c>
       <c r="AD125" t="n">
         <v>0</v>
       </c>
       <c r="AE125" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AF125" t="n">
         <v>0</v>
       </c>
       <c r="AG125" t="n">
-        <v>0.819309</v>
+        <v>1.5</v>
       </c>
       <c r="AH125"/>
       <c r="AI125"/>
@@ -14031,7 +14032,7 @@
         <v>0</v>
       </c>
       <c r="AL125" t="n">
-        <v>195291</v>
+        <v>179000</v>
       </c>
     </row>
     <row r="126">
@@ -14048,33 +14049,29 @@
         <v>41</v>
       </c>
       <c r="E126" t="s">
-        <v>228</v>
+        <v>49</v>
       </c>
       <c r="F126"/>
       <c r="G126" s="1" t="n">
-        <v>43251</v>
+        <v>43320</v>
       </c>
       <c r="H126" s="1" t="n">
-        <v>43263</v>
+        <v>43381</v>
       </c>
       <c r="I126" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="J126" t="s">
-        <v>230</v>
-      </c>
-      <c r="K126" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="L126" t="n">
-        <v>0.99</v>
-      </c>
+        <v>233</v>
+      </c>
+      <c r="K126"/>
+      <c r="L126"/>
       <c r="M126" t="n">
-        <v>0.20202</v>
+        <v>0.749971</v>
       </c>
       <c r="N126"/>
       <c r="O126" t="n">
-        <v>0.20202</v>
+        <v>0.749971</v>
       </c>
       <c r="P126" t="n">
         <v>1</v>
@@ -14119,16 +14116,16 @@
         <v>0</v>
       </c>
       <c r="AD126" t="n">
-        <v>0.20202</v>
+        <v>0</v>
       </c>
       <c r="AE126" t="n">
         <v>0</v>
       </c>
       <c r="AF126" t="n">
-        <v>0</v>
+        <v>0.749971</v>
       </c>
       <c r="AG126" t="n">
-        <v>0.20202</v>
+        <v>0.749971</v>
       </c>
       <c r="AH126"/>
       <c r="AI126"/>
@@ -14137,210 +14134,6 @@
         <v>0</v>
       </c>
       <c r="AL126" t="n">
-        <v>176336</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="s">
-        <v>38</v>
-      </c>
-      <c r="B127" t="s">
-        <v>39</v>
-      </c>
-      <c r="C127" t="s">
-        <v>40</v>
-      </c>
-      <c r="D127" t="s">
-        <v>41</v>
-      </c>
-      <c r="E127" t="s">
-        <v>49</v>
-      </c>
-      <c r="F127"/>
-      <c r="G127" s="1" t="n">
-        <v>43259</v>
-      </c>
-      <c r="H127" s="1" t="n">
-        <v>43332</v>
-      </c>
-      <c r="I127" t="s">
-        <v>231</v>
-      </c>
-      <c r="J127" t="s">
-        <v>232</v>
-      </c>
-      <c r="K127"/>
-      <c r="L127"/>
-      <c r="M127" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="N127"/>
-      <c r="O127" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="P127" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q127" t="n">
-        <v>0</v>
-      </c>
-      <c r="R127" t="n">
-        <v>0</v>
-      </c>
-      <c r="S127" t="n">
-        <v>0</v>
-      </c>
-      <c r="T127" t="n">
-        <v>0</v>
-      </c>
-      <c r="U127" t="n">
-        <v>0</v>
-      </c>
-      <c r="V127" t="n">
-        <v>0</v>
-      </c>
-      <c r="W127" t="n">
-        <v>0</v>
-      </c>
-      <c r="X127" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y127" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE127" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="AF127" t="n">
-        <v>0</v>
-      </c>
-      <c r="AG127" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="AH127"/>
-      <c r="AI127"/>
-      <c r="AJ127"/>
-      <c r="AK127" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL127" t="n">
-        <v>179000</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="s">
-        <v>38</v>
-      </c>
-      <c r="B128" t="s">
-        <v>39</v>
-      </c>
-      <c r="C128" t="s">
-        <v>40</v>
-      </c>
-      <c r="D128" t="s">
-        <v>41</v>
-      </c>
-      <c r="E128" t="s">
-        <v>49</v>
-      </c>
-      <c r="F128"/>
-      <c r="G128" s="1" t="n">
-        <v>43320</v>
-      </c>
-      <c r="H128" s="1" t="n">
-        <v>43381</v>
-      </c>
-      <c r="I128" t="s">
-        <v>233</v>
-      </c>
-      <c r="J128" t="s">
-        <v>234</v>
-      </c>
-      <c r="K128"/>
-      <c r="L128"/>
-      <c r="M128" t="n">
-        <v>0.749971</v>
-      </c>
-      <c r="N128"/>
-      <c r="O128" t="n">
-        <v>0.749971</v>
-      </c>
-      <c r="P128" t="n">
-        <v>1</v>
-      </c>
-      <c r="Q128" t="n">
-        <v>0</v>
-      </c>
-      <c r="R128" t="n">
-        <v>0</v>
-      </c>
-      <c r="S128" t="n">
-        <v>0</v>
-      </c>
-      <c r="T128" t="n">
-        <v>0</v>
-      </c>
-      <c r="U128" t="n">
-        <v>0</v>
-      </c>
-      <c r="V128" t="n">
-        <v>0</v>
-      </c>
-      <c r="W128" t="n">
-        <v>0</v>
-      </c>
-      <c r="X128" t="n">
-        <v>0</v>
-      </c>
-      <c r="Y128" t="n">
-        <v>0</v>
-      </c>
-      <c r="Z128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AA128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AB128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AC128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AD128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AE128" t="n">
-        <v>0</v>
-      </c>
-      <c r="AF128" t="n">
-        <v>0.749971</v>
-      </c>
-      <c r="AG128" t="n">
-        <v>0.749971</v>
-      </c>
-      <c r="AH128"/>
-      <c r="AI128"/>
-      <c r="AJ128"/>
-      <c r="AK128" t="b">
-        <v>0</v>
-      </c>
-      <c r="AL128" t="n">
         <v>181218</v>
       </c>
     </row>

</xml_diff>